<commit_message>
change format excel demo
</commit_message>
<xml_diff>
--- a/public/exports/pass-holders.xlsx
+++ b/public/exports/pass-holders.xlsx
@@ -116,10 +116,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="M/D/YYYY"/>
-    <numFmt numFmtId="166" formatCode="D\-MMM\-YY"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -218,10 +217,18 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -230,15 +237,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -263,14 +262,14 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="14.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.33"/>
@@ -280,49 +279,49 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="8.83"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="4" t="s">
         <v>13</v>
       </c>
       <c r="E2" s="4" t="s">
@@ -331,30 +330,30 @@
       <c r="F2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="4" t="s">
         <v>23</v>
       </c>
       <c r="E3" s="4" t="s">
@@ -366,13 +365,13 @@
       <c r="G3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="J3" s="4" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>